<commit_message>
Small edits to excel
</commit_message>
<xml_diff>
--- a/Feature_Explanations.xlsx
+++ b/Feature_Explanations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffen/Programs/Fico-Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6758F47-5348-B046-989A-86E70647AD33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723A2AD5-2FB8-734E-83ED-550A37207D48}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{178F9147-DF64-6F40-BAA4-73FF5D3D202A}"/>
   </bookViews>
@@ -221,9 +221,6 @@
   </si>
   <si>
     <t>Observations for Special Cases</t>
-  </si>
-  <si>
-    <t>Data is centred in the range 160-240. No correlation</t>
   </si>
   <si>
     <t>Slightly more negative in special case</t>
@@ -561,6 +558,9 @@
   </si>
   <si>
     <t xml:space="preserve">Positive correlation. Never delinquent is clearly the optimal. </t>
+  </si>
+  <si>
+    <t>Slight positive correlation. Data is centred in the range 160-240. Guassian type distribution</t>
   </si>
 </sst>
 </file>
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61F1D2D0-32BF-9A4F-BB53-291A2A833120}">
   <dimension ref="B1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1375,10 +1375,10 @@
         <v>23</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>136</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>137</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>55</v>
@@ -1452,7 +1452,7 @@
         <v>62</v>
       </c>
       <c r="M2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:16">
@@ -1487,10 +1487,10 @@
         <v>588</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1528,10 +1528,10 @@
         <v>588</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:16">
@@ -1566,10 +1566,10 @@
         <v>588</v>
       </c>
       <c r="L5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:16">
@@ -1604,10 +1604,10 @@
         <v>588</v>
       </c>
       <c r="L6" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" t="s">
         <v>72</v>
-      </c>
-      <c r="M6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="2:16">
@@ -1642,10 +1642,10 @@
         <v>588</v>
       </c>
       <c r="L7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="2:16">
@@ -1680,10 +1680,10 @@
         <v>588</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="2:16">
@@ -1718,10 +1718,10 @@
         <v>588</v>
       </c>
       <c r="L9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:16">
@@ -1756,13 +1756,13 @@
         <v>588</v>
       </c>
       <c r="L10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M10" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="N10" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1799,7 +1799,7 @@
         <v>588</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M11" s="23"/>
       <c r="N11" s="23"/>
@@ -1838,7 +1838,7 @@
         <v>588</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
@@ -1877,7 +1877,7 @@
         <v>588</v>
       </c>
       <c r="L13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:16">
@@ -1912,7 +1912,7 @@
         <v>588</v>
       </c>
       <c r="L14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:16">
@@ -1947,7 +1947,7 @@
         <v>588</v>
       </c>
       <c r="L15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:16">
@@ -1982,10 +1982,10 @@
         <v>588</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -2023,7 +2023,7 @@
         <v>588</v>
       </c>
       <c r="L17" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -2058,7 +2058,7 @@
         <v>588</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -2093,10 +2093,10 @@
         <v>588</v>
       </c>
       <c r="L19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="M19" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -2134,10 +2134,10 @@
         <v>588</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -2175,10 +2175,10 @@
         <v>588</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -2216,10 +2216,10 @@
         <v>588</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -2257,10 +2257,10 @@
         <v>588</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -2298,10 +2298,10 @@
         <v>588</v>
       </c>
       <c r="L24" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -2309,46 +2309,46 @@
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="2:16">
       <c r="B30" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="2:16">
       <c r="L31" s="28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="2:16">
       <c r="L32" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="8:12">
       <c r="L33" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="8:12">
@@ -2356,22 +2356,22 @@
     </row>
     <row r="35" spans="8:12">
       <c r="L35" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="8:12">
       <c r="L36" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="8:12">
       <c r="L37" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="8:12">
       <c r="H42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2397,7 +2397,7 @@
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" s="17"/>
     </row>
@@ -2412,17 +2412,17 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F3" s="13"/>
       <c r="J3" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="13"/>
@@ -2438,10 +2438,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2449,7 +2449,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
@@ -2457,11 +2457,11 @@
         <v>1</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="13"/>
       <c r="J5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -2469,7 +2469,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
@@ -2477,11 +2477,11 @@
         <v>2</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G6" s="13"/>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2489,7 +2489,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -2497,7 +2497,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="13"/>
     </row>
@@ -2506,7 +2506,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
@@ -2514,16 +2514,16 @@
         <v>4</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -2531,7 +2531,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -2539,7 +2539,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -2547,15 +2547,15 @@
         <v>6</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>107</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
@@ -2563,10 +2563,10 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2594,17 +2594,17 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
       <c r="E15" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F15" s="13"/>
       <c r="J15" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -2612,7 +2612,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2620,10 +2620,10 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -2631,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2639,11 +2639,11 @@
         <v>1</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G17" s="13"/>
       <c r="J17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -2651,7 +2651,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -2659,11 +2659,11 @@
         <v>2</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" s="13"/>
       <c r="J18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -2671,7 +2671,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2679,11 +2679,11 @@
         <v>3</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G19" s="13"/>
       <c r="J19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2691,7 +2691,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2699,11 +2699,11 @@
         <v>4</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" s="13"/>
       <c r="J20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2711,7 +2711,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2719,10 +2719,10 @@
         <v>5</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -2730,7 +2730,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2738,10 +2738,10 @@
         <v>6</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -2749,7 +2749,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -2757,13 +2757,13 @@
         <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -2771,13 +2771,13 @@
         <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="J24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -2794,7 +2794,7 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="G26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:10">

</xml_diff>